<commit_message>
ahora enviar los datos al backend se envian por el boton que se habia diseñado en un primer momento, los erroes que daba el sistema por id al generar elementos por map, fueron corregidos ahora los datos se envia juntamente con los del head y los del table
</commit_message>
<xml_diff>
--- a/app/api/data/plantilla.xlsx
+++ b/app/api/data/plantilla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBT\Documents\TBTapp\tbt-app\app\api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF1245A-E9CB-477A-9052-8D23A8C7AA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83B2610-6382-4ACA-98D1-AAF37F09EE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="3090" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="3075" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="requi" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t xml:space="preserve">O R D E N   D E   C O M P R A. </t>
   </si>
@@ -280,9 +280,6 @@
     <t>PARTE</t>
   </si>
   <si>
-    <t>CON: CPU-003</t>
-  </si>
-  <si>
     <t>Solicito.</t>
   </si>
   <si>
@@ -317,16 +314,28 @@
   </si>
   <si>
     <t>Gerente General</t>
+  </si>
+  <si>
+    <t>CON: CPU-005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TERRACERIAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-06-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provedor1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts>
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="20">
+  <fonts>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,8 +470,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills>
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,7 +505,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="95">
+  <borders>
     <border>
       <left/>
       <right/>
@@ -1784,11 +1799,95 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="249">
+  <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2120,27 +2219,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="17" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="10" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="10" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2150,33 +2228,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="10" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="10" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="7" fontId="10" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="10" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="91" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2186,9 +2237,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="10" fillId="0" borderId="91" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2214,6 +2262,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="9" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2238,113 +2367,170 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="9" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2367,169 +2553,129 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="91" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="95" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="96" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="97" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="17" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="10" fillId="0" borderId="99" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="10" fillId="0" borderId="96" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="97" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="98" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="100" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="100" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2837,16 +2983,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:V40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="140" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="123" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -2854,10 +2999,10 @@
     <col min="8" max="8" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" style="141" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="124" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="142" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.5703125" bestFit="1" customWidth="1"/>
@@ -2871,34 +3016,34 @@
     </row>
     <row r="2" spans="2:16" ht="20.25" customHeight="1">
       <c r="B2" s="91"/>
-      <c r="F2" s="143" t="s">
+      <c r="F2" t="s" s="153">
         <v>58</v>
       </c>
-      <c r="G2" s="143"/>
-      <c r="H2" s="143"/>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
-      <c r="K2" s="144"/>
-      <c r="L2" s="143"/>
-      <c r="M2" s="143"/>
-      <c r="N2" s="143"/>
-      <c r="O2" s="143"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
+      <c r="J2" s="153"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="153"/>
+      <c r="M2" s="153"/>
+      <c r="N2" s="153"/>
+      <c r="O2" s="153"/>
       <c r="P2" s="94"/>
     </row>
     <row r="3" spans="2:16" ht="35.25" customHeight="1">
       <c r="B3" s="91"/>
-      <c r="F3" s="145" t="s">
+      <c r="F3" t="s" s="155">
         <v>59</v>
       </c>
-      <c r="G3" s="145"/>
-      <c r="H3" s="145"/>
-      <c r="I3" s="145"/>
-      <c r="J3" s="145"/>
-      <c r="K3" s="146"/>
-      <c r="L3" s="145"/>
-      <c r="M3" s="145"/>
-      <c r="N3" s="145"/>
-      <c r="O3" s="145"/>
+      <c r="G3" s="155"/>
+      <c r="H3" s="155"/>
+      <c r="I3" s="155"/>
+      <c r="J3" s="155"/>
+      <c r="K3" s="156"/>
+      <c r="L3" s="155"/>
+      <c r="M3" s="155"/>
+      <c r="N3" s="155"/>
+      <c r="O3" s="155"/>
       <c r="P3" s="94"/>
     </row>
     <row r="4" spans="2:16" ht="7.5" customHeight="1">
@@ -2909,44 +3054,48 @@
     <row r="5" spans="2:16" ht="18.75" customHeight="1">
       <c r="B5" s="95"/>
       <c r="C5" s="96"/>
-      <c r="D5" s="147"/>
-      <c r="E5" s="147"/>
-      <c r="F5" s="147"/>
-      <c r="G5" s="147"/>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
-      <c r="K5" s="148"/>
-      <c r="L5" s="149" t="s">
+      <c r="D5" s="157"/>
+      <c r="E5" s="157"/>
+      <c r="F5" s="157"/>
+      <c r="G5" s="157"/>
+      <c r="H5" s="157"/>
+      <c r="I5" s="157"/>
+      <c r="J5" s="157"/>
+      <c r="K5" s="158"/>
+      <c r="L5" t="s" s="159">
         <v>60</v>
       </c>
-      <c r="M5" s="149"/>
-      <c r="N5" s="149"/>
-      <c r="O5" s="150"/>
-      <c r="P5" s="98"/>
+      <c r="M5" s="159"/>
+      <c r="N5" s="159"/>
+      <c r="O5" s="160"/>
+      <c r="P5" s="98">
+        <v>234</v>
+      </c>
     </row>
     <row r="6" spans="2:16" ht="18.75" customHeight="1">
       <c r="B6" s="91"/>
-      <c r="D6" s="147"/>
-      <c r="E6" s="147"/>
-      <c r="F6" s="147"/>
-      <c r="G6" s="147"/>
-      <c r="H6" s="147"/>
-      <c r="I6" s="147"/>
-      <c r="J6" s="147"/>
-      <c r="K6" s="148"/>
+      <c r="D6" s="157"/>
+      <c r="E6" s="157"/>
+      <c r="F6" s="157"/>
+      <c r="G6" s="157"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="157"/>
+      <c r="J6" s="157"/>
+      <c r="K6" s="158"/>
       <c r="L6" s="97"/>
       <c r="N6" s="93"/>
     </row>
     <row r="7" spans="2:16" ht="18.75" customHeight="1">
-      <c r="B7" s="99" t="s">
+      <c r="B7" t="s" s="99">
         <v>61</v>
       </c>
-      <c r="C7" s="151"/>
-      <c r="D7" s="151"/>
-      <c r="E7" s="151"/>
-      <c r="F7" s="151"/>
-      <c r="H7" s="100" t="s">
+      <c r="C7" s="150">
+        <v>2103</v>
+      </c>
+      <c r="D7" s="150"/>
+      <c r="E7" s="150"/>
+      <c r="F7" s="150"/>
+      <c r="H7" t="s" s="100">
         <v>62</v>
       </c>
       <c r="I7" s="101"/>
@@ -2954,19 +3103,19 @@
       <c r="K7" s="102"/>
       <c r="L7" s="101"/>
       <c r="M7" s="101"/>
-      <c r="N7" s="152" t="s">
+      <c r="N7" t="s" s="151">
         <v>63</v>
       </c>
-      <c r="O7" s="152"/>
-      <c r="P7" s="152"/>
+      <c r="O7" s="151"/>
+      <c r="P7" s="151"/>
     </row>
     <row r="8" spans="2:16" ht="12.75" customHeight="1">
       <c r="B8" s="99"/>
-      <c r="D8" s="153"/>
-      <c r="E8" s="153"/>
-      <c r="F8" s="153"/>
+      <c r="D8" s="128"/>
+      <c r="E8" s="128"/>
+      <c r="F8" s="128"/>
       <c r="H8" s="104"/>
-      <c r="I8" s="105" t="s">
+      <c r="I8" t="s" s="105">
         <v>64</v>
       </c>
       <c r="J8" s="105"/>
@@ -2974,20 +3123,22 @@
       <c r="N8" s="93"/>
     </row>
     <row r="9" spans="2:16" ht="18.75" customHeight="1">
-      <c r="B9" s="99" t="s">
+      <c r="B9" t="s" s="99">
         <v>65</v>
       </c>
-      <c r="C9" s="151"/>
-      <c r="D9" s="151"/>
-      <c r="E9" s="151"/>
-      <c r="F9" s="151"/>
+      <c r="C9" t="s" s="150">
+        <v>93</v>
+      </c>
+      <c r="D9" s="150"/>
+      <c r="E9" s="150"/>
+      <c r="F9" s="150"/>
       <c r="H9" s="104"/>
-      <c r="I9" s="105" t="s">
+      <c r="I9" t="s" s="105">
         <v>66</v>
       </c>
       <c r="J9" s="105"/>
       <c r="K9" s="92"/>
-      <c r="N9" s="105" t="s">
+      <c r="N9" t="s" s="105">
         <v>67</v>
       </c>
       <c r="P9" s="104"/>
@@ -2996,34 +3147,36 @@
       <c r="B10" s="99"/>
       <c r="C10" s="106"/>
       <c r="H10" s="104"/>
-      <c r="I10" s="105" t="s">
+      <c r="I10" t="s" s="105">
         <v>68</v>
       </c>
       <c r="J10" s="105"/>
       <c r="K10" s="92"/>
-      <c r="N10" s="105" t="s">
+      <c r="N10" t="s" s="105">
         <v>69</v>
       </c>
       <c r="P10" s="104"/>
     </row>
     <row r="11" spans="2:16" ht="18.75" customHeight="1">
-      <c r="B11" s="99" t="s">
+      <c r="B11" t="s" s="99">
         <v>70</v>
       </c>
-      <c r="C11" s="154"/>
-      <c r="D11" s="154"/>
-      <c r="E11" s="154"/>
-      <c r="F11" s="154"/>
-      <c r="G11" s="94" t="s">
+      <c r="C11" t="s" s="152">
+        <v>94</v>
+      </c>
+      <c r="D11" s="152"/>
+      <c r="E11" s="152"/>
+      <c r="F11" s="152"/>
+      <c r="G11" t="s" s="94">
         <v>33</v>
       </c>
       <c r="H11" s="104"/>
-      <c r="I11" s="105" t="s">
+      <c r="I11" t="s" s="105">
         <v>71</v>
       </c>
       <c r="J11" s="105"/>
       <c r="K11" s="92"/>
-      <c r="N11" s="105" t="s">
+      <c r="N11" t="s" s="105">
         <v>72</v>
       </c>
       <c r="P11" s="104"/>
@@ -3031,7 +3184,7 @@
     <row r="12" spans="2:16" ht="18.75" customHeight="1">
       <c r="B12" s="91"/>
       <c r="H12" s="104"/>
-      <c r="I12" s="105" t="s">
+      <c r="I12" t="s" s="105">
         <v>73</v>
       </c>
       <c r="J12" s="105"/>
@@ -3041,7 +3194,7 @@
     <row r="13" spans="2:16" ht="18.75" customHeight="1">
       <c r="B13" s="91"/>
       <c r="H13" s="104"/>
-      <c r="I13" s="105" t="s">
+      <c r="I13" t="s" s="105">
         <v>74</v>
       </c>
       <c r="J13" s="105"/>
@@ -3051,7 +3204,7 @@
     <row r="14" spans="2:16" ht="18.75" customHeight="1">
       <c r="B14" s="91"/>
       <c r="H14" s="104"/>
-      <c r="I14" s="105" t="s">
+      <c r="I14" t="s" s="105">
         <v>75</v>
       </c>
       <c r="J14" s="105"/>
@@ -3069,56 +3222,56 @@
       <c r="N16" s="93"/>
     </row>
     <row r="17" spans="2:22" ht="18.75" customHeight="1">
-      <c r="B17" s="155" t="s">
+      <c r="B17" t="s" s="146">
         <v>24</v>
       </c>
-      <c r="C17" s="107" t="s">
+      <c r="C17" t="s" s="107">
         <v>76</v>
       </c>
-      <c r="D17" s="157" t="s">
+      <c r="D17" t="s" s="137">
         <v>28</v>
       </c>
-      <c r="E17" s="158"/>
-      <c r="F17" s="158"/>
-      <c r="G17" s="158"/>
-      <c r="H17" s="159"/>
-      <c r="I17" s="157" t="s">
+      <c r="E17" s="138"/>
+      <c r="F17" s="138"/>
+      <c r="G17" s="138"/>
+      <c r="H17" s="139"/>
+      <c r="I17" t="s" s="137">
         <v>26</v>
       </c>
-      <c r="J17" s="163" t="s">
+      <c r="J17" t="s" s="135">
         <v>25</v>
       </c>
-      <c r="K17" s="165" t="s">
+      <c r="K17" t="s" s="148">
         <v>29</v>
       </c>
-      <c r="L17" s="163" t="s">
+      <c r="L17" t="s" s="135">
         <v>77</v>
       </c>
-      <c r="M17" s="157" t="s">
+      <c r="M17" t="s" s="137">
         <v>78</v>
       </c>
-      <c r="N17" s="158"/>
-      <c r="O17" s="158"/>
-      <c r="P17" s="159"/>
+      <c r="N17" s="138"/>
+      <c r="O17" s="138"/>
+      <c r="P17" s="139"/>
     </row>
     <row r="18" spans="2:22" ht="18.75" customHeight="1">
-      <c r="B18" s="156"/>
-      <c r="C18" s="108" t="s">
+      <c r="B18" s="147"/>
+      <c r="C18" t="s" s="108">
         <v>79</v>
       </c>
-      <c r="D18" s="160"/>
-      <c r="E18" s="161"/>
-      <c r="F18" s="161"/>
-      <c r="G18" s="161"/>
-      <c r="H18" s="162"/>
-      <c r="I18" s="160"/>
-      <c r="J18" s="164"/>
-      <c r="K18" s="166"/>
-      <c r="L18" s="164"/>
-      <c r="M18" s="160"/>
-      <c r="N18" s="161"/>
-      <c r="O18" s="161"/>
-      <c r="P18" s="162"/>
+      <c r="D18" s="140"/>
+      <c r="E18" s="141"/>
+      <c r="F18" s="141"/>
+      <c r="G18" s="141"/>
+      <c r="H18" s="142"/>
+      <c r="I18" s="140"/>
+      <c r="J18" s="136"/>
+      <c r="K18" s="149"/>
+      <c r="L18" s="136"/>
+      <c r="M18" s="140"/>
+      <c r="N18" s="141"/>
+      <c r="O18" s="141"/>
+      <c r="P18" s="142"/>
     </row>
     <row r="19" spans="2:22" ht="18.75" customHeight="1">
       <c r="B19" s="109"/>
@@ -3129,357 +3282,375 @@
       <c r="G19" s="110"/>
       <c r="H19" s="110"/>
       <c r="I19" s="110"/>
-      <c r="J19" s="110"/>
-      <c r="K19" s="111"/>
+      <c r="J19" s="249"/>
+      <c r="K19" s="259"/>
       <c r="L19" s="110"/>
       <c r="M19" s="110"/>
       <c r="N19" s="110"/>
       <c r="O19" s="110"/>
       <c r="P19" s="110"/>
     </row>
-    <row r="20" spans="2:22" ht="48" customHeight="1">
-      <c r="B20" s="112">
+    <row r="20" spans="2:22" ht="30" customHeight="1">
+      <c r="B20" s="223">
         <v>1</v>
       </c>
-      <c r="C20" s="113"/>
-      <c r="D20" s="167"/>
-      <c r="E20" s="168"/>
-      <c r="F20" s="168"/>
-      <c r="G20" s="168"/>
-      <c r="H20" s="169"/>
-      <c r="I20" s="114"/>
-      <c r="J20" s="115"/>
-      <c r="K20" s="116"/>
-      <c r="L20" s="117"/>
-      <c r="M20" s="170"/>
-      <c r="N20" s="171"/>
-      <c r="O20" s="171"/>
-      <c r="P20" s="172"/>
-    </row>
-    <row r="21" spans="2:22" ht="43.5" customHeight="1">
-      <c r="B21" s="121">
+      <c r="C20" s="224"/>
+      <c r="D20" s="225"/>
+      <c r="E20" s="226"/>
+      <c r="F20" s="226"/>
+      <c r="G20" s="226"/>
+      <c r="H20" s="227"/>
+      <c r="I20" s="245"/>
+      <c r="J20" s="250"/>
+      <c r="K20" s="260"/>
+      <c r="L20" t="s" s="255">
+        <v>95</v>
+      </c>
+      <c r="M20" s="129"/>
+      <c r="N20" s="130"/>
+      <c r="O20" s="130"/>
+      <c r="P20" s="131"/>
+    </row>
+    <row r="21" spans="2:22" ht="30" customHeight="1">
+      <c r="B21" s="228">
         <v>2</v>
       </c>
-      <c r="C21" s="122"/>
-      <c r="D21" s="173"/>
-      <c r="E21" s="174"/>
-      <c r="F21" s="174"/>
-      <c r="G21" s="174"/>
-      <c r="H21" s="175"/>
-      <c r="I21" s="122"/>
-      <c r="J21" s="123"/>
-      <c r="K21" s="124"/>
-      <c r="L21" s="122"/>
-      <c r="M21" s="176"/>
-      <c r="N21" s="177"/>
-      <c r="O21" s="177"/>
-      <c r="P21" s="178"/>
-    </row>
-    <row r="22" spans="2:22" ht="26.25" customHeight="1">
-      <c r="B22" s="121">
+      <c r="C21" s="229"/>
+      <c r="D21" s="230"/>
+      <c r="E21" s="231"/>
+      <c r="F21" s="231"/>
+      <c r="G21" s="231"/>
+      <c r="H21" s="232"/>
+      <c r="I21" s="246"/>
+      <c r="J21" s="251"/>
+      <c r="K21" s="261"/>
+      <c r="L21" s="256"/>
+      <c r="M21" s="143"/>
+      <c r="N21" s="144"/>
+      <c r="O21" s="144"/>
+      <c r="P21" s="145"/>
+    </row>
+    <row r="22" spans="2:22" ht="30" customHeight="1">
+      <c r="B22" s="228">
         <v>3</v>
       </c>
-      <c r="C22" s="122"/>
-      <c r="D22" s="170"/>
-      <c r="E22" s="171"/>
-      <c r="F22" s="171"/>
-      <c r="G22" s="171"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="122"/>
-      <c r="J22" s="123"/>
-      <c r="K22" s="124"/>
-      <c r="L22" s="122"/>
-      <c r="M22" s="179"/>
-      <c r="N22" s="180"/>
-      <c r="O22" s="180"/>
-      <c r="P22" s="181"/>
-    </row>
-    <row r="23" spans="2:22" ht="26.25" customHeight="1">
-      <c r="B23" s="121">
-        <f t="shared" ref="B23:B30" si="0">+B22+1</f>
-        <v>4</v>
-      </c>
-      <c r="C23" s="122"/>
-      <c r="D23" s="179"/>
-      <c r="E23" s="180"/>
-      <c r="F23" s="180"/>
-      <c r="G23" s="180"/>
-      <c r="H23" s="181"/>
-      <c r="I23" s="122"/>
-      <c r="J23" s="122"/>
-      <c r="K23" s="124"/>
-      <c r="L23" s="125"/>
-      <c r="M23" s="179"/>
-      <c r="N23" s="180"/>
-      <c r="O23" s="180"/>
-      <c r="P23" s="181"/>
-    </row>
-    <row r="24" spans="2:22" ht="25.5" customHeight="1">
-      <c r="B24" s="121">
+      <c r="C22" s="229"/>
+      <c r="D22" s="233"/>
+      <c r="E22" s="234"/>
+      <c r="F22" s="234"/>
+      <c r="G22" s="234"/>
+      <c r="H22" s="235"/>
+      <c r="I22" s="246"/>
+      <c r="J22" s="251"/>
+      <c r="K22" s="261"/>
+      <c r="L22" s="256"/>
+      <c r="M22" s="132"/>
+      <c r="N22" s="133"/>
+      <c r="O22" s="133"/>
+      <c r="P22" s="134"/>
+    </row>
+    <row r="23" spans="2:22" ht="30" customHeight="1">
+      <c r="B23" s="228">
+        <f t="shared" ref="B23:B27" si="0">+B22+1</f>
+      </c>
+      <c r="C23" s="229"/>
+      <c r="D23" s="236"/>
+      <c r="E23" s="237"/>
+      <c r="F23" s="237"/>
+      <c r="G23" s="237"/>
+      <c r="H23" s="238"/>
+      <c r="I23" s="246"/>
+      <c r="J23" s="252"/>
+      <c r="K23" s="261"/>
+      <c r="L23" s="257"/>
+      <c r="M23" s="132"/>
+      <c r="N23" s="133"/>
+      <c r="O23" s="133"/>
+      <c r="P23" s="134"/>
+    </row>
+    <row r="24" spans="2:22" ht="30" customHeight="1">
+      <c r="B24" s="228">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C24" s="122"/>
-      <c r="D24" s="179"/>
-      <c r="E24" s="180"/>
-      <c r="F24" s="180"/>
-      <c r="G24" s="180"/>
-      <c r="H24" s="181"/>
-      <c r="I24" s="122"/>
-      <c r="J24" s="122" t="s">
+      </c>
+      <c r="C24" s="229"/>
+      <c r="D24" s="236"/>
+      <c r="E24" s="237"/>
+      <c r="F24" s="237"/>
+      <c r="G24" s="237"/>
+      <c r="H24" s="238"/>
+      <c r="I24" s="246"/>
+      <c r="J24" s="253"/>
+      <c r="K24" s="262"/>
+      <c r="L24" s="257"/>
+      <c r="M24" s="132"/>
+      <c r="N24" s="133"/>
+      <c r="O24" s="133"/>
+      <c r="P24" s="134"/>
+    </row>
+    <row r="25" spans="2:22" ht="30" customHeight="1">
+      <c r="B25" s="228">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C25" s="229"/>
+      <c r="D25" s="236"/>
+      <c r="E25" s="237"/>
+      <c r="F25" s="237"/>
+      <c r="G25" s="237"/>
+      <c r="H25" s="238"/>
+      <c r="I25" s="246"/>
+      <c r="J25" s="252"/>
+      <c r="K25" s="261"/>
+      <c r="L25" s="257"/>
+      <c r="M25" s="132"/>
+      <c r="N25" s="133"/>
+      <c r="O25" s="133"/>
+      <c r="P25" s="134"/>
+    </row>
+    <row r="26" spans="2:22" ht="30" customHeight="1">
+      <c r="B26" s="228">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C26" s="229"/>
+      <c r="D26" s="236"/>
+      <c r="E26" s="237"/>
+      <c r="F26" s="237"/>
+      <c r="G26" s="237"/>
+      <c r="H26" s="238"/>
+      <c r="I26" s="246"/>
+      <c r="J26" s="264"/>
+      <c r="K26" s="265"/>
+      <c r="L26" s="257"/>
+      <c r="M26" s="132"/>
+      <c r="N26" s="133"/>
+      <c r="O26" s="133"/>
+      <c r="P26" s="134"/>
+    </row>
+    <row r="27" spans="2:22" ht="30" customHeight="1">
+      <c r="B27" s="228">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C27" s="239"/>
+      <c r="D27" s="233"/>
+      <c r="E27" s="234"/>
+      <c r="F27" s="234"/>
+      <c r="G27" s="234"/>
+      <c r="H27" s="235"/>
+      <c r="I27" s="247"/>
+      <c r="J27" s="253"/>
+      <c r="K27" s="262"/>
+      <c r="L27" t="s" s="257">
+        <v>33</v>
+      </c>
+      <c r="M27" s="132"/>
+      <c r="N27" s="133"/>
+      <c r="O27" s="133"/>
+      <c r="P27" s="134"/>
+    </row>
+    <row r="28" spans="2:22" ht="30" customHeight="1">
+      <c r="B28" s="228"/>
+      <c r="C28" s="239"/>
+      <c r="D28" s="233"/>
+      <c r="E28" s="234"/>
+      <c r="F28" s="234"/>
+      <c r="G28" s="234"/>
+      <c r="H28" s="235"/>
+      <c r="I28" s="247"/>
+      <c r="J28" t="s" s="252">
         <v>48</v>
       </c>
-      <c r="K24" s="124">
+      <c r="K28" s="261">
         <f>SUM(K20:K22)</f>
-        <v>0</v>
-      </c>
-      <c r="L24" s="125"/>
-      <c r="M24" s="179"/>
-      <c r="N24" s="180"/>
-      <c r="O24" s="180"/>
-      <c r="P24" s="181"/>
-    </row>
-    <row r="25" spans="2:22" ht="21" customHeight="1">
-      <c r="B25" s="121">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C25" s="122"/>
-      <c r="D25" s="179"/>
-      <c r="E25" s="180"/>
-      <c r="F25" s="180"/>
-      <c r="G25" s="180"/>
-      <c r="H25" s="181"/>
-      <c r="I25" s="122"/>
-      <c r="J25" s="122"/>
-      <c r="K25" s="124"/>
-      <c r="L25" s="125"/>
-      <c r="M25" s="179"/>
-      <c r="N25" s="180"/>
-      <c r="O25" s="180"/>
-      <c r="P25" s="181"/>
-    </row>
-    <row r="26" spans="2:22" ht="20.100000000000001" customHeight="1">
-      <c r="B26" s="121">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C26" s="122"/>
-      <c r="D26" s="179"/>
-      <c r="E26" s="180"/>
-      <c r="F26" s="180"/>
-      <c r="G26" s="180"/>
-      <c r="H26" s="181"/>
-      <c r="I26" s="122"/>
-      <c r="J26" s="125"/>
-      <c r="K26" s="124"/>
-      <c r="L26" s="125"/>
-      <c r="M26" s="179"/>
-      <c r="N26" s="180"/>
-      <c r="O26" s="180"/>
-      <c r="P26" s="181"/>
-    </row>
-    <row r="27" spans="2:22" ht="20.100000000000001" customHeight="1">
-      <c r="B27" s="121">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C27" s="125"/>
-      <c r="D27" s="170" t="s">
+      </c>
+      <c r="L28" s="257"/>
+      <c r="M28" s="132"/>
+      <c r="N28" s="133"/>
+      <c r="O28" s="133"/>
+      <c r="P28" s="134"/>
+    </row>
+    <row r="29" spans="2:22" ht="30" customHeight="1">
+      <c r="B29" s="228"/>
+      <c r="C29" s="239"/>
+      <c r="D29" t="s" s="233">
+        <v>92</v>
+      </c>
+      <c r="E29" s="234"/>
+      <c r="F29" s="234"/>
+      <c r="G29" s="234"/>
+      <c r="H29" s="235"/>
+      <c r="I29" s="247"/>
+      <c r="J29" t="s" s="252">
+        <v>50</v>
+      </c>
+      <c r="K29" s="261">
+        <f>K28*0.16</f>
+      </c>
+      <c r="L29" s="257"/>
+      <c r="M29" s="111"/>
+      <c r="N29" s="112"/>
+      <c r="O29" s="112"/>
+      <c r="P29" s="113"/>
+    </row>
+    <row r="30" spans="2:22" ht="30" customHeight="1">
+      <c r="B30" s="240"/>
+      <c r="C30" s="241"/>
+      <c r="D30" s="242"/>
+      <c r="E30" s="243"/>
+      <c r="F30" s="243"/>
+      <c r="G30" s="243"/>
+      <c r="H30" s="244"/>
+      <c r="I30" s="248"/>
+      <c r="J30" s="254"/>
+      <c r="K30" s="263"/>
+      <c r="L30" s="258"/>
+      <c r="M30" t="s" s="114">
+        <v>33</v>
+      </c>
+      <c r="N30" s="115"/>
+      <c r="O30" s="115"/>
+      <c r="P30" s="116"/>
+    </row>
+    <row r="31" spans="2:22" ht="18.75" customHeight="1">
+      <c r="B31" s="117"/>
+      <c r="C31" s="118"/>
+      <c r="D31" s="118"/>
+      <c r="E31" s="118"/>
+      <c r="F31" s="118"/>
+      <c r="G31" s="118"/>
+      <c r="H31" s="118"/>
+      <c r="I31" s="118"/>
+      <c r="J31" s="118"/>
+      <c r="K31" s="119">
+        <f>K28+K29</f>
+      </c>
+      <c r="L31" s="118"/>
+      <c r="M31" s="118"/>
+      <c r="N31" s="120"/>
+      <c r="O31" s="118"/>
+      <c r="P31" s="118"/>
+      <c r="Q31" s="118"/>
+      <c r="R31" s="118"/>
+      <c r="S31" s="118"/>
+      <c r="T31" s="118"/>
+      <c r="U31" s="118"/>
+      <c r="V31" s="118"/>
+    </row>
+    <row r="32" spans="2:22" ht="18.75" customHeight="1">
+      <c r="B32" t="s" s="127">
         <v>80</v>
       </c>
-      <c r="E27" s="171"/>
-      <c r="F27" s="171"/>
-      <c r="G27" s="171"/>
-      <c r="H27" s="172"/>
-      <c r="I27" s="125"/>
-      <c r="J27" s="122" t="s">
-        <v>50</v>
-      </c>
-      <c r="K27" s="124">
-        <f>K24*0.16</f>
-        <v>0</v>
-      </c>
-      <c r="L27" s="125" t="s">
-        <v>33</v>
-      </c>
-      <c r="M27" s="179"/>
-      <c r="N27" s="180"/>
-      <c r="O27" s="180"/>
-      <c r="P27" s="181"/>
-    </row>
-    <row r="28" spans="2:22" ht="20.100000000000001" customHeight="1">
-      <c r="B28" s="121">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C28" s="125"/>
-      <c r="D28" s="170"/>
-      <c r="E28" s="171"/>
-      <c r="F28" s="171"/>
-      <c r="G28" s="171"/>
-      <c r="H28" s="172"/>
-      <c r="I28" s="125"/>
-      <c r="J28" s="125"/>
-      <c r="K28" s="126"/>
-      <c r="L28" s="125"/>
-      <c r="M28" s="179"/>
-      <c r="N28" s="180"/>
-      <c r="O28" s="180"/>
-      <c r="P28" s="181"/>
-    </row>
-    <row r="29" spans="2:22" ht="20.100000000000001" customHeight="1">
-      <c r="B29" s="121">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C29" s="125"/>
-      <c r="D29" s="170"/>
-      <c r="E29" s="171"/>
-      <c r="F29" s="171"/>
-      <c r="G29" s="171"/>
-      <c r="H29" s="172"/>
-      <c r="I29" s="125"/>
-      <c r="J29" s="125"/>
-      <c r="K29" s="127"/>
-      <c r="L29" s="125"/>
-      <c r="M29" s="118"/>
-      <c r="N29" s="119"/>
-      <c r="O29" s="119"/>
-      <c r="P29" s="120"/>
-    </row>
-    <row r="30" spans="2:22" ht="19.5" customHeight="1">
-      <c r="B30" s="128">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C30" s="129"/>
-      <c r="D30" s="182"/>
-      <c r="E30" s="183"/>
-      <c r="F30" s="183"/>
-      <c r="G30" s="183"/>
-      <c r="H30" s="184"/>
-      <c r="I30" s="129"/>
-      <c r="J30" s="129"/>
-      <c r="K30" s="133"/>
-      <c r="L30" s="129"/>
-      <c r="M30" s="130" t="s">
-        <v>33</v>
-      </c>
-      <c r="N30" s="131"/>
-      <c r="O30" s="131"/>
-      <c r="P30" s="132"/>
-    </row>
-    <row r="31" spans="2:22" ht="18.75" customHeight="1">
-      <c r="B31" s="134"/>
-      <c r="C31" s="135"/>
-      <c r="D31" s="135"/>
-      <c r="E31" s="135"/>
-      <c r="F31" s="135"/>
-      <c r="G31" s="135"/>
-      <c r="H31" s="135"/>
-      <c r="I31" s="135"/>
-      <c r="J31" s="135"/>
-      <c r="K31" s="136">
-        <f>K24+K27</f>
-        <v>0</v>
-      </c>
-      <c r="L31" s="135"/>
-      <c r="M31" s="135"/>
-      <c r="N31" s="137"/>
-      <c r="O31" s="135"/>
-      <c r="P31" s="135"/>
-      <c r="Q31" s="135"/>
-      <c r="R31" s="135"/>
-      <c r="S31" s="135"/>
-      <c r="T31" s="135"/>
-      <c r="U31" s="135"/>
-      <c r="V31" s="135"/>
-    </row>
-    <row r="32" spans="2:22" ht="18.75" customHeight="1">
-      <c r="B32" s="185" t="s">
+      <c r="C32" s="128"/>
+      <c r="F32" t="s" s="94">
         <v>81</v>
       </c>
-      <c r="C32" s="153"/>
-      <c r="F32" s="94" t="s">
+      <c r="K32" t="s" s="121">
         <v>82</v>
       </c>
-      <c r="K32" s="138" t="s">
+      <c r="N32" t="s" s="103">
         <v>83</v>
-      </c>
-      <c r="N32" s="103" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="33" spans="2:15" ht="18.75" customHeight="1">
       <c r="B33" s="91"/>
-      <c r="K33" s="138"/>
+      <c r="K33" s="121"/>
       <c r="N33" s="103"/>
     </row>
     <row r="34" spans="2:15" ht="18.75" customHeight="1">
       <c r="B34" s="91"/>
-      <c r="K34" s="138"/>
+      <c r="K34" s="121"/>
       <c r="N34" s="103"/>
     </row>
     <row r="35" spans="2:15" ht="18.75" customHeight="1">
       <c r="B35" s="91"/>
-      <c r="K35" s="138"/>
+      <c r="K35" s="121"/>
       <c r="N35" s="103"/>
     </row>
     <row r="36" spans="2:15" ht="18.75" customHeight="1">
       <c r="B36" s="91"/>
-      <c r="K36" s="138"/>
+      <c r="K36" s="121"/>
       <c r="N36" s="103"/>
     </row>
     <row r="37" spans="2:15" ht="17.25" customHeight="1">
       <c r="B37" s="91"/>
-      <c r="K37" s="138"/>
+      <c r="K37" s="121"/>
       <c r="N37" s="103"/>
     </row>
     <row r="38" spans="2:15" ht="18.75" customHeight="1">
-      <c r="B38" s="139" t="s">
+      <c r="B38" t="s" s="122">
+        <v>84</v>
+      </c>
+      <c r="E38" t="s" s="126">
         <v>85</v>
       </c>
-      <c r="E38" s="186" t="s">
+      <c r="F38" s="126"/>
+      <c r="G38" s="126"/>
+      <c r="H38" s="126"/>
+      <c r="J38" t="s" s="94">
         <v>86</v>
       </c>
-      <c r="F38" s="186"/>
-      <c r="G38" s="186"/>
-      <c r="H38" s="186"/>
-      <c r="J38" s="94" t="s">
+      <c r="K38" s="121"/>
+      <c r="N38" t="s" s="103">
         <v>87</v>
       </c>
-      <c r="K38" s="138"/>
-      <c r="N38" s="103" t="s">
+    </row>
+    <row r="39" spans="2:15" ht="18.75" customHeight="1">
+      <c r="B39" t="s" s="127">
         <v>88</v>
       </c>
-    </row>
-    <row r="39" spans="2:15" ht="18.75" customHeight="1">
-      <c r="B39" s="185" t="s">
+      <c r="C39" s="128"/>
+      <c r="F39" t="s" s="103">
         <v>89</v>
       </c>
-      <c r="C39" s="153"/>
-      <c r="F39" s="103" t="s">
+      <c r="G39" s="94"/>
+      <c r="J39" t="s" s="94">
         <v>90</v>
       </c>
-      <c r="G39" s="94"/>
-      <c r="J39" s="94" t="s">
+      <c r="K39" s="121"/>
+      <c r="M39" s="94"/>
+      <c r="N39" t="s" s="103">
         <v>91</v>
-      </c>
-      <c r="K39" s="138"/>
-      <c r="M39" s="94"/>
-      <c r="N39" s="103" t="s">
-        <v>92</v>
       </c>
       <c r="O39" s="94"/>
     </row>
     <row r="40" spans="2:15" ht="18.75" customHeight="1">
       <c r="B40" s="91"/>
-      <c r="K40" s="138"/>
+      <c r="K40" s="121"/>
       <c r="N40" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="F2:O2"/>
+    <mergeCell ref="F3:O3"/>
+    <mergeCell ref="D5:K5"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="D6:K6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="M17:P18"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="M23:P23"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="M26:P26"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="M27:P27"/>
     <mergeCell ref="E38:H38"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="D28:H28"/>
@@ -3487,40 +3658,8 @@
     <mergeCell ref="D29:H29"/>
     <mergeCell ref="D30:H30"/>
     <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="M26:P26"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="M22:P22"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="M23:P23"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="M17:P18"/>
-    <mergeCell ref="D20:H20"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="M21:P21"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="F2:O2"/>
-    <mergeCell ref="F3:O3"/>
-    <mergeCell ref="D5:K5"/>
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="D6:K6"/>
   </mergeCells>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3530,9 +3669,8 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A6" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3556,24 +3694,24 @@
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="187" t="s">
+      <c r="E1" t="s" s="216">
         <v>0</v>
       </c>
-      <c r="F1" s="187"/>
-      <c r="G1" s="187"/>
-      <c r="H1" s="187"/>
-      <c r="I1" s="187"/>
-      <c r="J1" s="187"/>
-      <c r="K1" s="187"/>
+      <c r="F1" s="216"/>
+      <c r="G1" s="216"/>
+      <c r="H1" s="216"/>
+      <c r="I1" s="216"/>
+      <c r="J1" s="216"/>
+      <c r="K1" s="216"/>
       <c r="L1" s="4"/>
-      <c r="M1" s="5" t="s">
+      <c r="M1" t="s" s="5">
         <v>1</v>
       </c>
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1">
       <c r="B2" s="6"/>
-      <c r="L2" s="8" t="s">
+      <c r="L2" t="s" s="8">
         <v>2</v>
       </c>
       <c r="M2" s="9"/>
@@ -3581,132 +3719,132 @@
     <row r="3" spans="1:14" ht="18.75" customHeight="1">
       <c r="B3" s="10"/>
       <c r="K3" s="11"/>
-      <c r="L3" s="12" t="s">
+      <c r="L3" t="s" s="12">
         <v>3</v>
       </c>
       <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:14" ht="12.75" customHeight="1">
-      <c r="B4" s="14" t="s">
+      <c r="B4" t="s" s="14">
         <v>4</v>
       </c>
-      <c r="C4" s="188" t="s">
+      <c r="C4" t="s" s="217">
         <v>5</v>
       </c>
-      <c r="D4" s="188"/>
-      <c r="E4" s="188"/>
-      <c r="F4" s="189"/>
-      <c r="G4" s="15" t="s">
+      <c r="D4" s="217"/>
+      <c r="E4" s="217"/>
+      <c r="F4" s="218"/>
+      <c r="G4" t="s" s="15">
         <v>6</v>
       </c>
-      <c r="H4" s="190"/>
-      <c r="I4" s="190"/>
-      <c r="J4" s="190"/>
-      <c r="K4" s="191"/>
-      <c r="L4" s="16" t="s">
+      <c r="H4" s="219"/>
+      <c r="I4" s="219"/>
+      <c r="J4" s="219"/>
+      <c r="K4" s="220"/>
+      <c r="L4" t="s" s="16">
         <v>7</v>
       </c>
       <c r="M4" s="17"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1">
-      <c r="B5" s="18" t="s">
+      <c r="B5" t="s" s="18">
         <v>8</v>
       </c>
-      <c r="C5" s="192" t="s">
+      <c r="C5" t="s" s="221">
         <v>9</v>
       </c>
-      <c r="D5" s="192"/>
-      <c r="E5" s="192"/>
-      <c r="F5" s="193"/>
-      <c r="G5" s="19" t="s">
+      <c r="D5" s="221"/>
+      <c r="E5" s="221"/>
+      <c r="F5" s="222"/>
+      <c r="G5" t="s" s="19">
         <v>10</v>
       </c>
-      <c r="H5" s="194"/>
-      <c r="I5" s="194"/>
-      <c r="J5" s="194"/>
-      <c r="K5" s="195"/>
-      <c r="L5" s="196"/>
-      <c r="M5" s="197"/>
+      <c r="H5" s="212"/>
+      <c r="I5" s="212"/>
+      <c r="J5" s="212"/>
+      <c r="K5" s="213"/>
+      <c r="L5" s="208"/>
+      <c r="M5" s="209"/>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1">
-      <c r="B6" s="198" t="s">
+      <c r="B6" t="s" s="210">
         <v>11</v>
       </c>
-      <c r="C6" s="199"/>
-      <c r="D6" s="199"/>
-      <c r="E6" s="199"/>
-      <c r="F6" s="200"/>
-      <c r="G6" s="19" t="s">
+      <c r="C6" s="196"/>
+      <c r="D6" s="196"/>
+      <c r="E6" s="196"/>
+      <c r="F6" s="211"/>
+      <c r="G6" t="s" s="19">
         <v>12</v>
       </c>
-      <c r="H6" s="194"/>
-      <c r="I6" s="194"/>
-      <c r="J6" s="194"/>
-      <c r="K6" s="195"/>
-      <c r="L6" s="23" t="s">
+      <c r="H6" s="212"/>
+      <c r="I6" s="212"/>
+      <c r="J6" s="212"/>
+      <c r="K6" s="213"/>
+      <c r="L6" t="s" s="23">
         <v>13</v>
       </c>
       <c r="M6" s="24"/>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1">
-      <c r="B7" s="18" t="s">
+      <c r="B7" t="s" s="18">
         <v>14</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" t="s" s="21">
         <v>15</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
       <c r="F7" s="22"/>
-      <c r="G7" s="19" t="s">
+      <c r="G7" t="s" s="19">
         <v>16</v>
       </c>
-      <c r="H7" s="194"/>
-      <c r="I7" s="194"/>
-      <c r="J7" s="194"/>
-      <c r="K7" s="195"/>
-      <c r="L7" s="201"/>
-      <c r="M7" s="202"/>
+      <c r="H7" s="212"/>
+      <c r="I7" s="212"/>
+      <c r="J7" s="212"/>
+      <c r="K7" s="213"/>
+      <c r="L7" s="214"/>
+      <c r="M7" s="215"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
-      <c r="B8" s="18" t="s">
+      <c r="B8" t="s" s="18">
         <v>17</v>
       </c>
-      <c r="C8" s="199"/>
-      <c r="D8" s="199"/>
-      <c r="E8" s="199"/>
-      <c r="F8" s="199"/>
-      <c r="G8" s="203" t="s">
+      <c r="C8" s="196"/>
+      <c r="D8" s="196"/>
+      <c r="E8" s="196"/>
+      <c r="F8" s="196"/>
+      <c r="G8" t="s" s="197">
         <v>18</v>
       </c>
-      <c r="H8" s="204"/>
-      <c r="I8" s="205" t="s">
+      <c r="H8" s="198"/>
+      <c r="I8" t="s" s="199">
         <v>19</v>
       </c>
-      <c r="J8" s="206"/>
-      <c r="K8" s="207"/>
-      <c r="L8" s="23" t="s">
+      <c r="J8" s="200"/>
+      <c r="K8" s="201"/>
+      <c r="L8" t="s" s="23">
         <v>20</v>
       </c>
       <c r="M8" s="29"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1">
-      <c r="B9" s="208"/>
-      <c r="C9" s="209"/>
-      <c r="D9" s="209"/>
-      <c r="E9" s="209"/>
-      <c r="F9" s="210"/>
-      <c r="G9" s="211" t="s">
+      <c r="B9" s="202"/>
+      <c r="C9" s="203"/>
+      <c r="D9" s="203"/>
+      <c r="E9" s="203"/>
+      <c r="F9" s="204"/>
+      <c r="G9" t="s" s="205">
         <v>21</v>
       </c>
-      <c r="H9" s="212"/>
-      <c r="I9" s="212" t="s">
+      <c r="H9" s="206"/>
+      <c r="I9" t="s" s="206">
         <v>22</v>
       </c>
-      <c r="J9" s="212"/>
-      <c r="K9" s="213"/>
-      <c r="L9" s="214"/>
-      <c r="M9" s="215"/>
+      <c r="J9" s="206"/>
+      <c r="K9" s="207"/>
+      <c r="L9" s="186"/>
+      <c r="M9" s="187"/>
     </row>
     <row r="10" spans="1:14" ht="19.5" customHeight="1">
       <c r="B10" s="32"/>
@@ -3714,13 +3852,13 @@
       <c r="D10" s="33"/>
       <c r="E10" s="33"/>
       <c r="F10" s="34"/>
-      <c r="G10" s="35" t="s">
+      <c r="G10" t="s" s="35">
         <v>23</v>
       </c>
-      <c r="H10" s="216"/>
-      <c r="I10" s="216"/>
-      <c r="J10" s="216"/>
-      <c r="K10" s="217"/>
+      <c r="H10" s="188"/>
+      <c r="I10" s="188"/>
+      <c r="J10" s="188"/>
+      <c r="K10" s="189"/>
       <c r="L10" s="35"/>
       <c r="M10" s="36"/>
     </row>
@@ -3739,30 +3877,30 @@
       <c r="M11" s="38"/>
     </row>
     <row r="12" spans="1:14" ht="18.75" customHeight="1">
-      <c r="B12" s="39" t="s">
+      <c r="B12" t="s" s="39">
         <v>24</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" t="s" s="40">
         <v>25</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" t="s" s="40">
         <v>26</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" t="s" s="40">
         <v>27</v>
       </c>
-      <c r="F12" s="218" t="s">
+      <c r="F12" t="s" s="190">
         <v>28</v>
       </c>
-      <c r="G12" s="219"/>
-      <c r="H12" s="219"/>
-      <c r="I12" s="219"/>
-      <c r="J12" s="219"/>
-      <c r="K12" s="220"/>
-      <c r="L12" s="40" t="s">
+      <c r="G12" s="191"/>
+      <c r="H12" s="191"/>
+      <c r="I12" s="191"/>
+      <c r="J12" s="191"/>
+      <c r="K12" s="192"/>
+      <c r="L12" t="s" s="40">
         <v>29</v>
       </c>
-      <c r="M12" s="41" t="s">
+      <c r="M12" t="s" s="41">
         <v>30</v>
       </c>
     </row>
@@ -3770,16 +3908,16 @@
       <c r="B13" s="42"/>
       <c r="C13" s="43"/>
       <c r="D13" s="43"/>
-      <c r="E13" s="44" t="s">
+      <c r="E13" t="s" s="44">
         <v>31</v>
       </c>
-      <c r="F13" s="221"/>
-      <c r="G13" s="222"/>
-      <c r="H13" s="222"/>
-      <c r="I13" s="222"/>
-      <c r="J13" s="222"/>
-      <c r="K13" s="223"/>
-      <c r="L13" s="44" t="s">
+      <c r="F13" s="193"/>
+      <c r="G13" s="194"/>
+      <c r="H13" s="194"/>
+      <c r="I13" s="194"/>
+      <c r="J13" s="194"/>
+      <c r="K13" s="195"/>
+      <c r="L13" t="s" s="44">
         <v>32</v>
       </c>
       <c r="M13" s="46"/>
@@ -3789,16 +3927,15 @@
       <c r="C14" s="45"/>
       <c r="D14" s="44"/>
       <c r="E14" s="44"/>
-      <c r="F14" s="224"/>
-      <c r="G14" s="225"/>
-      <c r="H14" s="225"/>
-      <c r="I14" s="225"/>
-      <c r="J14" s="225"/>
-      <c r="K14" s="226"/>
+      <c r="F14" s="177"/>
+      <c r="G14" s="178"/>
+      <c r="H14" s="178"/>
+      <c r="I14" s="178"/>
+      <c r="J14" s="178"/>
+      <c r="K14" s="179"/>
       <c r="L14" s="50"/>
       <c r="M14" s="51">
         <f>+C14*L14</f>
-        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1">
@@ -3806,12 +3943,12 @@
       <c r="C15" s="45"/>
       <c r="D15" s="44"/>
       <c r="E15" s="44"/>
-      <c r="F15" s="224"/>
-      <c r="G15" s="225"/>
-      <c r="H15" s="225"/>
-      <c r="I15" s="225"/>
-      <c r="J15" s="225"/>
-      <c r="K15" s="226"/>
+      <c r="F15" s="177"/>
+      <c r="G15" s="178"/>
+      <c r="H15" s="178"/>
+      <c r="I15" s="178"/>
+      <c r="J15" s="178"/>
+      <c r="K15" s="179"/>
       <c r="L15" s="50"/>
       <c r="M15" s="51"/>
     </row>
@@ -3820,12 +3957,12 @@
       <c r="C16" s="53"/>
       <c r="D16" s="44"/>
       <c r="E16" s="44"/>
-      <c r="F16" s="227"/>
-      <c r="G16" s="228"/>
-      <c r="H16" s="228"/>
-      <c r="I16" s="228"/>
-      <c r="J16" s="228"/>
-      <c r="K16" s="229"/>
+      <c r="F16" s="180"/>
+      <c r="G16" s="181"/>
+      <c r="H16" s="181"/>
+      <c r="I16" s="181"/>
+      <c r="J16" s="181"/>
+      <c r="K16" s="182"/>
       <c r="L16" s="50"/>
       <c r="M16" s="51"/>
     </row>
@@ -3834,12 +3971,12 @@
       <c r="C17" s="53"/>
       <c r="D17" s="44"/>
       <c r="E17" s="54"/>
-      <c r="F17" s="224"/>
-      <c r="G17" s="225"/>
-      <c r="H17" s="225"/>
-      <c r="I17" s="225"/>
-      <c r="J17" s="225"/>
-      <c r="K17" s="226"/>
+      <c r="F17" s="177"/>
+      <c r="G17" s="178"/>
+      <c r="H17" s="178"/>
+      <c r="I17" s="178"/>
+      <c r="J17" s="178"/>
+      <c r="K17" s="179"/>
       <c r="L17" s="50"/>
       <c r="M17" s="51"/>
     </row>
@@ -3848,12 +3985,12 @@
       <c r="C18" s="53"/>
       <c r="D18" s="44"/>
       <c r="E18" s="54"/>
-      <c r="F18" s="224"/>
-      <c r="G18" s="225"/>
-      <c r="H18" s="225"/>
-      <c r="I18" s="225"/>
-      <c r="J18" s="225"/>
-      <c r="K18" s="226"/>
+      <c r="F18" s="177"/>
+      <c r="G18" s="178"/>
+      <c r="H18" s="178"/>
+      <c r="I18" s="178"/>
+      <c r="J18" s="178"/>
+      <c r="K18" s="179"/>
       <c r="L18" s="50"/>
       <c r="M18" s="51"/>
     </row>
@@ -3862,14 +3999,14 @@
       <c r="C19" s="53"/>
       <c r="D19" s="44"/>
       <c r="E19" s="44"/>
-      <c r="F19" s="224" t="s">
+      <c r="F19" t="s" s="177">
         <v>33</v>
       </c>
-      <c r="G19" s="225"/>
-      <c r="H19" s="225"/>
-      <c r="I19" s="225"/>
-      <c r="J19" s="225"/>
-      <c r="K19" s="226"/>
+      <c r="G19" s="178"/>
+      <c r="H19" s="178"/>
+      <c r="I19" s="178"/>
+      <c r="J19" s="178"/>
+      <c r="K19" s="179"/>
       <c r="L19" s="50"/>
       <c r="M19" s="51"/>
     </row>
@@ -3878,14 +4015,14 @@
       <c r="C20" s="53"/>
       <c r="D20" s="44"/>
       <c r="E20" s="44"/>
-      <c r="F20" s="224" t="s">
+      <c r="F20" t="s" s="177">
         <v>33</v>
       </c>
-      <c r="G20" s="225"/>
-      <c r="H20" s="225"/>
-      <c r="I20" s="225"/>
-      <c r="J20" s="225"/>
-      <c r="K20" s="226"/>
+      <c r="G20" s="178"/>
+      <c r="H20" s="178"/>
+      <c r="I20" s="178"/>
+      <c r="J20" s="178"/>
+      <c r="K20" s="179"/>
       <c r="L20" s="50"/>
       <c r="M20" s="51"/>
     </row>
@@ -3894,12 +4031,12 @@
       <c r="C21" s="53"/>
       <c r="D21" s="44"/>
       <c r="E21" s="44"/>
-      <c r="F21" s="224"/>
-      <c r="G21" s="225"/>
-      <c r="H21" s="225"/>
-      <c r="I21" s="225"/>
-      <c r="J21" s="225"/>
-      <c r="K21" s="226"/>
+      <c r="F21" s="177"/>
+      <c r="G21" s="178"/>
+      <c r="H21" s="178"/>
+      <c r="I21" s="178"/>
+      <c r="J21" s="178"/>
+      <c r="K21" s="179"/>
       <c r="L21" s="50"/>
       <c r="M21" s="51"/>
     </row>
@@ -3919,12 +4056,12 @@
       <c r="C23" s="53"/>
       <c r="D23" s="44"/>
       <c r="E23" s="44"/>
-      <c r="F23" s="227"/>
-      <c r="G23" s="228"/>
-      <c r="H23" s="228"/>
-      <c r="I23" s="228"/>
-      <c r="J23" s="228"/>
-      <c r="K23" s="229"/>
+      <c r="F23" s="180"/>
+      <c r="G23" s="181"/>
+      <c r="H23" s="181"/>
+      <c r="I23" s="181"/>
+      <c r="J23" s="181"/>
+      <c r="K23" s="182"/>
       <c r="L23" s="50"/>
       <c r="M23" s="51"/>
     </row>
@@ -3933,12 +4070,12 @@
       <c r="C24" s="53"/>
       <c r="D24" s="27"/>
       <c r="E24" s="44"/>
-      <c r="F24" s="224"/>
-      <c r="G24" s="225"/>
-      <c r="H24" s="225"/>
-      <c r="I24" s="225"/>
-      <c r="J24" s="225"/>
-      <c r="K24" s="226"/>
+      <c r="F24" s="177"/>
+      <c r="G24" s="178"/>
+      <c r="H24" s="178"/>
+      <c r="I24" s="178"/>
+      <c r="J24" s="178"/>
+      <c r="K24" s="179"/>
       <c r="L24" s="50"/>
       <c r="M24" s="51"/>
     </row>
@@ -3949,7 +4086,7 @@
       <c r="E25" s="57"/>
       <c r="F25" s="28"/>
       <c r="G25" s="30"/>
-      <c r="H25" s="30" t="s">
+      <c r="H25" t="s" s="30">
         <v>34</v>
       </c>
       <c r="I25" s="30"/>
@@ -3965,7 +4102,7 @@
       <c r="E26" s="27"/>
       <c r="F26" s="28"/>
       <c r="G26" s="60"/>
-      <c r="H26" s="30" t="s">
+      <c r="H26" t="s" s="30">
         <v>35</v>
       </c>
       <c r="I26" s="30"/>
@@ -3981,7 +4118,7 @@
       <c r="E27" s="43"/>
       <c r="F27" s="61"/>
       <c r="G27" s="30"/>
-      <c r="H27" s="30" t="s">
+      <c r="H27" t="s" s="30">
         <v>36</v>
       </c>
       <c r="I27" s="62"/>
@@ -3992,14 +4129,14 @@
     </row>
     <row r="28" spans="2:13" ht="15" customHeight="1">
       <c r="B28" s="52"/>
-      <c r="C28" s="28" t="s">
+      <c r="C28" t="s" s="28">
         <v>37</v>
       </c>
       <c r="D28" s="27"/>
       <c r="E28" s="64"/>
       <c r="F28" s="28"/>
       <c r="G28" s="31"/>
-      <c r="H28" s="31" t="s">
+      <c r="H28" t="s" s="31">
         <v>38</v>
       </c>
       <c r="I28" s="30"/>
@@ -4009,7 +4146,7 @@
       <c r="M28" s="59"/>
     </row>
     <row r="29" spans="2:13" ht="18.75" customHeight="1">
-      <c r="B29" s="52" t="s">
+      <c r="B29" t="s" s="52">
         <v>33</v>
       </c>
       <c r="C29" s="25"/>
@@ -4017,69 +4154,69 @@
       <c r="E29" s="43"/>
       <c r="F29" s="25"/>
       <c r="G29" s="31"/>
-      <c r="H29" s="31" t="s">
+      <c r="H29" t="s" s="31">
         <v>39</v>
       </c>
       <c r="I29" s="66"/>
       <c r="J29" s="31"/>
       <c r="K29" s="63"/>
       <c r="L29" s="58"/>
-      <c r="M29" s="67" t="s">
+      <c r="M29" t="s" s="67">
         <v>33</v>
       </c>
     </row>
     <row r="30" spans="2:13" ht="15" customHeight="1">
       <c r="B30" s="52"/>
       <c r="C30" s="27"/>
-      <c r="D30" s="68" t="s">
+      <c r="D30" t="s" s="68">
         <v>33</v>
       </c>
       <c r="E30" s="64"/>
-      <c r="F30" s="28" t="s">
+      <c r="F30" t="s" s="28">
         <v>40</v>
       </c>
       <c r="G30" s="30"/>
-      <c r="H30" s="30" t="s">
+      <c r="H30" t="s" s="30">
         <v>41</v>
       </c>
       <c r="I30" s="30"/>
       <c r="J30" s="30"/>
       <c r="K30" s="26"/>
       <c r="L30" s="58"/>
-      <c r="M30" s="67" t="s">
+      <c r="M30" t="s" s="67">
         <v>33</v>
       </c>
     </row>
     <row r="31" spans="2:13" ht="12.75" customHeight="1">
-      <c r="B31" s="230" t="s">
+      <c r="B31" t="s" s="183">
         <v>42</v>
       </c>
-      <c r="C31" s="231"/>
-      <c r="D31" s="231"/>
-      <c r="E31" s="231"/>
-      <c r="F31" s="231"/>
-      <c r="G31" s="231"/>
-      <c r="H31" s="231"/>
-      <c r="I31" s="231"/>
-      <c r="J31" s="231"/>
-      <c r="K31" s="232"/>
+      <c r="C31" s="184"/>
+      <c r="D31" s="184"/>
+      <c r="E31" s="184"/>
+      <c r="F31" s="184"/>
+      <c r="G31" s="184"/>
+      <c r="H31" s="184"/>
+      <c r="I31" s="184"/>
+      <c r="J31" s="184"/>
+      <c r="K31" s="185"/>
       <c r="L31" s="58"/>
-      <c r="M31" s="67" t="s">
+      <c r="M31" t="s" s="67">
         <v>33</v>
       </c>
     </row>
     <row r="32" spans="2:13" ht="18.75" customHeight="1">
-      <c r="B32" s="69" t="s">
+      <c r="B32" t="s" s="69">
         <v>33</v>
       </c>
-      <c r="C32" s="48" t="s">
+      <c r="C32" t="s" s="48">
         <v>33</v>
       </c>
-      <c r="D32" s="48" t="s">
+      <c r="D32" t="s" s="48">
         <v>33</v>
       </c>
       <c r="E32" s="48"/>
-      <c r="F32" s="48" t="s">
+      <c r="F32" t="s" s="48">
         <v>33</v>
       </c>
       <c r="G32" s="48"/>
@@ -4087,55 +4224,54 @@
       <c r="I32" s="48"/>
       <c r="J32" s="48"/>
       <c r="K32" s="49"/>
-      <c r="L32" s="70" t="s">
+      <c r="L32" t="s" s="70">
         <v>33</v>
       </c>
-      <c r="M32" s="67" t="s">
+      <c r="M32" t="s" s="67">
         <v>33</v>
       </c>
     </row>
     <row r="33" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B33" s="233" t="str">
+      <c r="B33" s="174">
         <f>+C4</f>
-        <v>TRITURADOS BASALTICOS TEPETLAOXTOC, S.A DE C.V</v>
-      </c>
-      <c r="C33" s="234"/>
-      <c r="D33" s="234"/>
-      <c r="E33" s="234"/>
-      <c r="F33" s="234"/>
-      <c r="G33" s="234"/>
-      <c r="H33" s="234"/>
-      <c r="I33" s="234"/>
-      <c r="J33" s="235"/>
+      </c>
+      <c r="C33" s="175"/>
+      <c r="D33" s="175"/>
+      <c r="E33" s="175"/>
+      <c r="F33" s="175"/>
+      <c r="G33" s="175"/>
+      <c r="H33" s="175"/>
+      <c r="I33" s="175"/>
+      <c r="J33" s="176"/>
       <c r="K33" s="30"/>
-      <c r="L33" s="70" t="s">
+      <c r="L33" t="s" s="70">
         <v>33</v>
       </c>
-      <c r="M33" s="67" t="s">
+      <c r="M33" t="s" s="67">
         <v>33</v>
       </c>
     </row>
     <row r="34" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B34" s="233" t="s">
+      <c r="B34" t="s" s="174">
         <v>43</v>
       </c>
-      <c r="C34" s="234"/>
-      <c r="D34" s="235"/>
-      <c r="E34" s="234" t="s">
+      <c r="C34" s="175"/>
+      <c r="D34" s="176"/>
+      <c r="E34" t="s" s="175">
         <v>44</v>
       </c>
-      <c r="F34" s="234"/>
-      <c r="G34" s="235"/>
-      <c r="H34" s="234" t="s">
+      <c r="F34" s="175"/>
+      <c r="G34" s="176"/>
+      <c r="H34" t="s" s="175">
         <v>45</v>
       </c>
-      <c r="I34" s="234"/>
-      <c r="J34" s="235"/>
+      <c r="I34" s="175"/>
+      <c r="J34" s="176"/>
       <c r="K34" s="30"/>
-      <c r="L34" s="70" t="s">
+      <c r="L34" t="s" s="70">
         <v>33</v>
       </c>
-      <c r="M34" s="67" t="s">
+      <c r="M34" t="s" s="67">
         <v>33</v>
       </c>
     </row>
@@ -4196,47 +4332,45 @@
       <c r="M38" s="59"/>
     </row>
     <row r="39" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B39" s="236"/>
-      <c r="C39" s="237"/>
-      <c r="D39" s="238"/>
-      <c r="E39" s="237" t="s">
+      <c r="B39" s="161"/>
+      <c r="C39" s="162"/>
+      <c r="D39" s="163"/>
+      <c r="E39" t="s" s="162">
         <v>46</v>
       </c>
-      <c r="F39" s="237"/>
-      <c r="G39" s="238"/>
-      <c r="H39" s="237" t="s">
+      <c r="F39" s="162"/>
+      <c r="G39" s="163"/>
+      <c r="H39" t="s" s="162">
         <v>47</v>
       </c>
-      <c r="I39" s="237"/>
-      <c r="J39" s="238"/>
+      <c r="I39" s="162"/>
+      <c r="J39" s="163"/>
       <c r="K39" s="81"/>
-      <c r="L39" s="27" t="s">
+      <c r="L39" t="s" s="27">
         <v>48</v>
       </c>
       <c r="M39" s="59">
         <f>SUM(M14:M38)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B40" s="236" t="s">
+      <c r="B40" t="s" s="161">
         <v>49</v>
       </c>
-      <c r="C40" s="237"/>
-      <c r="D40" s="237"/>
-      <c r="E40" s="237"/>
-      <c r="F40" s="237"/>
-      <c r="G40" s="237"/>
-      <c r="H40" s="237"/>
-      <c r="I40" s="237"/>
-      <c r="J40" s="238"/>
+      <c r="C40" s="162"/>
+      <c r="D40" s="162"/>
+      <c r="E40" s="162"/>
+      <c r="F40" s="162"/>
+      <c r="G40" s="162"/>
+      <c r="H40" s="162"/>
+      <c r="I40" s="162"/>
+      <c r="J40" s="163"/>
       <c r="K40" s="82"/>
-      <c r="L40" s="27" t="s">
+      <c r="L40" t="s" s="27">
         <v>50</v>
       </c>
       <c r="M40" s="59">
         <f>M39*0.16</f>
-        <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:14" ht="18.75" customHeight="1">
@@ -4250,7 +4384,7 @@
       <c r="I41" s="72"/>
       <c r="J41" s="84"/>
       <c r="K41" s="82"/>
-      <c r="L41" s="27" t="s">
+      <c r="L41" t="s" s="27">
         <v>51</v>
       </c>
       <c r="M41" s="59"/>
@@ -4259,45 +4393,44 @@
       <c r="B42" s="77"/>
       <c r="C42" s="37"/>
       <c r="D42" s="37"/>
-      <c r="E42" s="239" t="s">
+      <c r="E42" t="s" s="164">
         <v>52</v>
       </c>
-      <c r="F42" s="240"/>
-      <c r="G42" s="241"/>
-      <c r="H42" s="242"/>
-      <c r="I42" s="242"/>
-      <c r="J42" s="243"/>
+      <c r="F42" s="165"/>
+      <c r="G42" s="166"/>
+      <c r="H42" s="167"/>
+      <c r="I42" s="167"/>
+      <c r="J42" s="168"/>
       <c r="K42" s="82"/>
-      <c r="L42" s="27" t="s">
+      <c r="L42" t="s" s="27">
         <v>53</v>
       </c>
       <c r="M42" s="59"/>
     </row>
     <row r="43" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B43" s="244" t="s">
+      <c r="B43" t="s" s="169">
         <v>54</v>
       </c>
-      <c r="C43" s="245"/>
-      <c r="D43" s="245"/>
-      <c r="E43" s="246" t="s">
+      <c r="C43" s="170"/>
+      <c r="D43" s="170"/>
+      <c r="E43" t="s" s="171">
         <v>55</v>
       </c>
-      <c r="F43" s="245"/>
-      <c r="G43" s="247"/>
-      <c r="H43" s="245" t="s">
+      <c r="F43" s="170"/>
+      <c r="G43" s="172"/>
+      <c r="H43" t="s" s="170">
         <v>56</v>
       </c>
-      <c r="I43" s="245"/>
-      <c r="J43" s="248"/>
-      <c r="K43" s="85" t="s">
+      <c r="I43" s="170"/>
+      <c r="J43" s="173"/>
+      <c r="K43" t="s" s="85">
         <v>33</v>
       </c>
-      <c r="L43" s="86" t="s">
+      <c r="L43" t="s" s="86">
         <v>57</v>
       </c>
       <c r="M43" s="87">
         <f>+M39+M40-M41-M42</f>
-        <v>0</v>
       </c>
       <c r="N43" s="88"/>
     </row>
@@ -4317,49 +4450,49 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="F12:K13"/>
+    <mergeCell ref="F14:K14"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="F20:K20"/>
+    <mergeCell ref="F21:K21"/>
+    <mergeCell ref="F23:K23"/>
+    <mergeCell ref="F24:K24"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="B33:J33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:J39"/>
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="E42:G42"/>
     <mergeCell ref="H42:J42"/>
     <mergeCell ref="B43:D43"/>
     <mergeCell ref="E43:G43"/>
     <mergeCell ref="H43:J43"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="F21:K21"/>
-    <mergeCell ref="F23:K23"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="B33:J33"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="F19:K19"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="F12:K13"/>
-    <mergeCell ref="F14:K14"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="H5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>